<commit_message>
More edits to template
</commit_message>
<xml_diff>
--- a/src/templates/template.xlsx
+++ b/src/templates/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brandon/GradeScope-Importer/src/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B98FC8-FD4F-404D-8828-77833AEA9A9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6AEFC6-D04C-E345-B312-B67D1CEA4C19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -421,7 +421,7 @@
   <dimension ref="B2:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -444,7 +444,7 @@
         <v>1</v>
       </c>
       <c r="H3" t="str">
-        <f>IF(SUM($C$35:$H$35) &lt;&gt; 0,SUM($C$34:$H$34)/SUM($C$35:$H$35),"")</f>
+        <f>IF(SUM($C$35:$H$35) &lt;&gt; 0,100*SUM($C$35:$H$35),"")</f>
         <v/>
       </c>
     </row>
@@ -504,27 +504,27 @@
         <v>7</v>
       </c>
       <c r="C35" t="str">
-        <f t="shared" ref="C35:H35" si="0">IF(COUNT(C8:C33)&lt;&gt;0,C7,"")</f>
+        <f>IF(COUNT(C8:C33)&lt;&gt;0,COUNT(C8:C33)*C7,"")</f>
         <v/>
       </c>
       <c r="D35" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(COUNT(D8:D33)&lt;&gt;0,COUNT(D8:D33)*D7,"")</f>
         <v/>
       </c>
       <c r="E35" t="str">
-        <f>IF(COUNT(E8:E33)&lt;&gt;0,E7,"")</f>
+        <f>IF(COUNT(E8:E33)&lt;&gt;0,COUNT(E8:E33)*E7,"")</f>
         <v/>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(COUNT(F8:F33)&lt;&gt;0,COUNT(F8:F33)*F7,"")</f>
         <v/>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(COUNT(G8:G33)&lt;&gt;0,COUNT(G8:G33)*G7,"")</f>
         <v/>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(COUNT(H8:H33)&lt;&gt;0,COUNT(H8:H33)*H7,"")</f>
         <v/>
       </c>
     </row>

</xml_diff>